<commit_message>
More information updated to both excel documents
</commit_message>
<xml_diff>
--- a/Wire Harness/Connector Profile.xlsx
+++ b/Wire Harness/Connector Profile.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franklin.320\Buckeye Current\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14140" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="25620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="97">
   <si>
     <t>Connector Schematic No.</t>
   </si>
@@ -192,12 +197,6 @@
     <t>Thorttle Enable</t>
   </si>
   <si>
-    <t>Microfit</t>
-  </si>
-  <si>
-    <t>Coolant Pump 1</t>
-  </si>
-  <si>
     <t>Coolant Pump 2</t>
   </si>
   <si>
@@ -264,15 +263,6 @@
     <t>Pheonix Contact</t>
   </si>
   <si>
-    <t>USB</t>
-  </si>
-  <si>
-    <t>2-Circuit</t>
-  </si>
-  <si>
-    <t>6-Circuit</t>
-  </si>
-  <si>
     <t>Number of Positions</t>
   </si>
   <si>
@@ -291,9 +281,6 @@
     <t>Vendor Part No.</t>
   </si>
   <si>
-    <t>Not a connector?</t>
-  </si>
-  <si>
     <t>NTC M12-H</t>
   </si>
   <si>
@@ -307,13 +294,34 @@
   </si>
   <si>
     <t xml:space="preserve">AMP 114-18063-076 </t>
+  </si>
+  <si>
+    <t>43025-0200</t>
+  </si>
+  <si>
+    <t>43025-0400</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>Microfit 3.0 Receptable Housing, Dual Row, 2 Circuits, Halogen Free</t>
+  </si>
+  <si>
+    <t>Microfit 3.0 Receptable Housing, Dual Row, 4 Circuits, Halogen Free</t>
+  </si>
+  <si>
+    <t>Coolant Pump 1 (Motor Side)</t>
+  </si>
+  <si>
+    <t>USB?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -416,7 +424,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -430,6 +438,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -478,6 +489,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -806,22 +825,22 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.625" customWidth="1"/>
     <col min="2" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
-    <col min="6" max="6" width="34.5" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.875" customWidth="1"/>
+    <col min="4" max="4" width="18.125" customWidth="1"/>
+    <col min="5" max="5" width="22.875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="56.625" customWidth="1"/>
+    <col min="7" max="7" width="14.625" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20">
+    <row r="1" spans="1:8" ht="21">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -835,16 +854,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -858,13 +877,13 @@
         <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2">
+        <v>76</v>
+      </c>
+      <c r="E2" s="7">
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -878,13 +897,13 @@
         <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3">
+        <v>76</v>
+      </c>
+      <c r="E3" s="7">
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -898,13 +917,13 @@
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4">
+        <v>76</v>
+      </c>
+      <c r="E4" s="7">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -914,14 +933,17 @@
       <c r="B5" t="s">
         <v>41</v>
       </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
       <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5">
+        <v>92</v>
+      </c>
+      <c r="E5" s="7">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -935,13 +957,13 @@
         <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6">
+        <v>76</v>
+      </c>
+      <c r="E6" s="7">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -955,13 +977,13 @@
         <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7">
+        <v>76</v>
+      </c>
+      <c r="E7" s="7">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -972,16 +994,16 @@
         <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8">
+        <v>76</v>
+      </c>
+      <c r="E8" s="7">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -992,16 +1014,16 @@
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9">
+        <v>76</v>
+      </c>
+      <c r="E9" s="7">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1012,16 +1034,16 @@
         <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10">
+        <v>76</v>
+      </c>
+      <c r="E10" s="7">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1032,16 +1054,16 @@
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11">
+        <v>76</v>
+      </c>
+      <c r="E11" s="7">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1051,14 +1073,17 @@
       <c r="B12" t="s">
         <v>50</v>
       </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
       <c r="D12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12">
+        <v>92</v>
+      </c>
+      <c r="E12" s="7">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1068,6 +1093,18 @@
       <c r="B13" t="s">
         <v>51</v>
       </c>
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="7">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
@@ -1076,6 +1113,18 @@
       <c r="B14" t="s">
         <v>52</v>
       </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
@@ -1085,16 +1134,16 @@
         <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15">
+        <v>81</v>
+      </c>
+      <c r="E15" s="7">
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1105,16 +1154,16 @@
         <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16">
+        <v>81</v>
+      </c>
+      <c r="E16" s="7">
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1127,6 +1176,15 @@
       <c r="C17" t="s">
         <v>90</v>
       </c>
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
@@ -1135,16 +1193,25 @@
       <c r="B18" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>95</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="7">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1152,7 +1219,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1160,16 +1227,19 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21">
-        <v>6</v>
+        <v>92</v>
+      </c>
+      <c r="E21" s="7">
+        <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1177,16 +1247,19 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22">
-        <v>6</v>
+        <v>92</v>
+      </c>
+      <c r="E22" s="7">
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1194,15 +1267,15 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23">
+        <v>81</v>
+      </c>
+      <c r="E23" s="7">
         <v>3</v>
       </c>
     </row>
@@ -1211,10 +1284,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1222,15 +1295,15 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25">
+        <v>81</v>
+      </c>
+      <c r="E25" s="7">
         <v>63</v>
       </c>
     </row>
@@ -1239,19 +1312,19 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26">
+        <v>76</v>
+      </c>
+      <c r="E26" s="7">
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1259,16 +1332,19 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27">
+        <v>92</v>
+      </c>
+      <c r="E27" s="7">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1276,13 +1352,16 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
+      </c>
+      <c r="E28" s="7">
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1290,19 +1369,19 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1">
         <v>1542761</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29">
+        <v>78</v>
+      </c>
+      <c r="E29" s="7">
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1310,19 +1389,19 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C30" s="1">
         <v>1542761</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E30">
+        <v>78</v>
+      </c>
+      <c r="E30" s="7">
         <v>5</v>
       </c>
       <c r="F30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1330,19 +1409,19 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C31" s="1">
         <v>1542761</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31">
+        <v>78</v>
+      </c>
+      <c r="E31" s="7">
         <v>5</v>
       </c>
       <c r="F31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1350,19 +1429,19 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1">
         <v>1542761</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32">
+        <v>78</v>
+      </c>
+      <c r="E32" s="7">
         <v>5</v>
       </c>
       <c r="F32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1370,19 +1449,19 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="1">
         <v>1542761</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33">
+        <v>78</v>
+      </c>
+      <c r="E33" s="7">
         <v>5</v>
       </c>
       <c r="F33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1390,22 +1469,22 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" s="1">
         <v>1542761</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34">
+        <v>78</v>
+      </c>
+      <c r="E34" s="7">
         <v>5</v>
       </c>
       <c r="F34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="16">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="C35" s="3"/>
       <c r="F35" s="6"/>
     </row>

</xml_diff>